<commit_message>
radiobutton working, need dicision apl., speed of work
</commit_message>
<xml_diff>
--- a/files/eq_files/80001841.xlsx
+++ b/files/eq_files/80001841.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
   <si>
     <t>дата</t>
   </si>
@@ -90,6 +90,60 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>buffer txt file</t>
+  </si>
+  <si>
+    <t>buffer txt file 2</t>
+  </si>
+  <si>
+    <t>механічна поломка</t>
+  </si>
+  <si>
+    <t>електрична поломка</t>
+  </si>
+  <si>
+    <t>scaner</t>
+  </si>
+  <si>
+    <t>CPU 2000</t>
+  </si>
+  <si>
+    <t>СPU 2000</t>
+  </si>
+  <si>
+    <t>інший тип простою</t>
+  </si>
+  <si>
+    <t>налаштування принтера</t>
+  </si>
+  <si>
+    <t>втулочний модуль</t>
+  </si>
+  <si>
+    <t>налаштування втулочного модуля</t>
+  </si>
+  <si>
+    <t>ПЗ</t>
+  </si>
+  <si>
+    <t>ТО обладнання</t>
+  </si>
+  <si>
+    <t>механічне налаштування</t>
+  </si>
+  <si>
+    <t>заміна запчастин</t>
+  </si>
+  <si>
+    <t>налаштування симетричності розрізу</t>
+  </si>
+  <si>
+    <t>ТО аплікатора</t>
+  </si>
+  <si>
+    <t>очікування тех.відділу</t>
   </si>
   <si>
     <t>crimper wire</t>
@@ -50484,10 +50538,286 @@
       <c r="C97" t="s">
         <v>23</v>
       </c>
-      <c r="D97" t="s"/>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" t="s">
+        <v>18</v>
+      </c>
+      <c r="B98" t="s">
+        <v>19</v>
+      </c>
+      <c r="C98" t="s">
+        <v>23</v>
+      </c>
+      <c r="D98" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" t="s">
+        <v>18</v>
+      </c>
+      <c r="B99" t="s">
+        <v>19</v>
+      </c>
+      <c r="C99" t="s">
+        <v>23</v>
+      </c>
+      <c r="D99" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" t="s">
+        <v>18</v>
+      </c>
+      <c r="B100" t="s">
+        <v>12</v>
+      </c>
+      <c r="C100" t="s">
+        <v>14</v>
+      </c>
+      <c r="D100" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" t="s">
+        <v>18</v>
+      </c>
+      <c r="B101" t="s">
+        <v>12</v>
+      </c>
+      <c r="C101" t="s">
+        <v>14</v>
+      </c>
+      <c r="D101" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" t="s">
+        <v>18</v>
+      </c>
+      <c r="B102" t="s">
+        <v>12</v>
+      </c>
+      <c r="C102" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" t="s">
+        <v>18</v>
+      </c>
+      <c r="B103" t="s">
+        <v>12</v>
+      </c>
+      <c r="C103" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" t="s">
+        <v>18</v>
+      </c>
+      <c r="B104" t="s">
+        <v>12</v>
+      </c>
+      <c r="C104" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" t="s">
+        <v>18</v>
+      </c>
+      <c r="B105" t="s">
+        <v>12</v>
+      </c>
+      <c r="C105" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" t="s">
+        <v>18</v>
+      </c>
+      <c r="B106" t="s">
+        <v>12</v>
+      </c>
+      <c r="C106" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" t="s">
+        <v>18</v>
+      </c>
+      <c r="B107" t="s">
+        <v>12</v>
+      </c>
+      <c r="C107" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" t="s">
+        <v>18</v>
+      </c>
+      <c r="B108" t="s">
+        <v>12</v>
+      </c>
+      <c r="C108" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" t="s">
+        <v>18</v>
+      </c>
+      <c r="B109" t="s">
+        <v>12</v>
+      </c>
+      <c r="C109" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" t="s">
+        <v>18</v>
+      </c>
+      <c r="B110" t="s">
+        <v>12</v>
+      </c>
+      <c r="C110" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" t="s">
+        <v>18</v>
+      </c>
+      <c r="B111" t="s">
+        <v>12</v>
+      </c>
+      <c r="C111" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" t="s">
+        <v>18</v>
+      </c>
+      <c r="B112" t="s">
+        <v>12</v>
+      </c>
+      <c r="C112" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" t="s">
+        <v>18</v>
+      </c>
+      <c r="B113" t="s">
+        <v>12</v>
+      </c>
+      <c r="C113" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114" t="s">
+        <v>18</v>
+      </c>
+      <c r="B114" t="s">
+        <v>12</v>
+      </c>
+      <c r="C114" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" t="s">
+        <v>18</v>
+      </c>
+      <c r="B115" t="s">
+        <v>12</v>
+      </c>
+      <c r="C115" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116" t="s">
+        <v>18</v>
+      </c>
+      <c r="B116" t="s">
+        <v>12</v>
+      </c>
+      <c r="C116" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" t="s">
+        <v>18</v>
+      </c>
+      <c r="B117" t="s">
+        <v>12</v>
+      </c>
+      <c r="C117" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118" t="s">
+        <v>18</v>
+      </c>
+      <c r="B118" t="s">
+        <v>12</v>
+      </c>
+      <c r="C118" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119" t="s">
+        <v>18</v>
+      </c>
+      <c r="B119" t="s">
+        <v>12</v>
+      </c>
+      <c r="C119" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" t="s">
+        <v>18</v>
+      </c>
+      <c r="B120" t="s">
+        <v>12</v>
+      </c>
+      <c r="C120" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121" t="s">
+        <v>18</v>
+      </c>
+      <c r="B121" t="s">
+        <v>12</v>
+      </c>
+      <c r="C121" t="s">
+        <v>42</v>
+      </c>
+      <c r="D121" t="s"/>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122" t="s">
         <v>6</v>
       </c>
     </row>
@@ -50501,7 +50831,7 @@
         <v>400001370</v>
       </c>
       <c r="B1992" s="16" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C1992" s="13" t="n">
         <v>119000</v>
@@ -50512,7 +50842,7 @@
         <v>400001964</v>
       </c>
       <c r="B1993" s="16" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C1993" s="13" t="n">
         <v>120000</v>

</xml_diff>

<commit_message>
force speed write data
</commit_message>
<xml_diff>
--- a/files/eq_files/80001841.xlsx
+++ b/files/eq_files/80001841.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="56">
   <si>
     <t>дата</t>
   </si>
@@ -153,6 +153,30 @@
   </si>
   <si>
     <t>05/07/2018</t>
+  </si>
+  <si>
+    <t>23/07/2018</t>
+  </si>
+  <si>
+    <t>24/07/2018</t>
+  </si>
+  <si>
+    <t>testttt</t>
+  </si>
+  <si>
+    <t>25/07/2018</t>
+  </si>
+  <si>
+    <t>tesst</t>
+  </si>
+  <si>
+    <t>tt</t>
+  </si>
+  <si>
+    <t>test with summary of week data</t>
+  </si>
+  <si>
+    <t>test of data sent applicator</t>
   </si>
   <si>
     <t>crimper wire</t>
@@ -50868,6 +50892,229 @@
     </row>
     <row r="125" spans="1:5">
       <c r="A125" t="s">
+        <v>46</v>
+      </c>
+      <c r="B125" t="s">
+        <v>12</v>
+      </c>
+      <c r="C125" t="s">
+        <v>42</v>
+      </c>
+      <c r="D125" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126" t="s">
+        <v>47</v>
+      </c>
+      <c r="B126" t="s">
+        <v>12</v>
+      </c>
+      <c r="C126" t="s">
+        <v>38</v>
+      </c>
+      <c r="D126" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127" t="s">
+        <v>47</v>
+      </c>
+      <c r="B127" t="s">
+        <v>12</v>
+      </c>
+      <c r="C127" t="s">
+        <v>38</v>
+      </c>
+      <c r="D127" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128" t="s">
+        <v>49</v>
+      </c>
+      <c r="B128" t="s">
+        <v>12</v>
+      </c>
+      <c r="C128" t="s">
+        <v>36</v>
+      </c>
+      <c r="D128" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129" t="s">
+        <v>49</v>
+      </c>
+      <c r="B129" t="s">
+        <v>12</v>
+      </c>
+      <c r="C129" t="s">
+        <v>32</v>
+      </c>
+      <c r="D129" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130" t="s">
+        <v>49</v>
+      </c>
+      <c r="B130" t="s">
+        <v>12</v>
+      </c>
+      <c r="C130" t="s">
+        <v>32</v>
+      </c>
+      <c r="D130" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
+      <c r="A131" t="s">
+        <v>49</v>
+      </c>
+      <c r="B131" t="s">
+        <v>12</v>
+      </c>
+      <c r="C131" t="s">
+        <v>32</v>
+      </c>
+      <c r="D131" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="A132" t="s">
+        <v>49</v>
+      </c>
+      <c r="B132" t="s">
+        <v>19</v>
+      </c>
+      <c r="C132" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
+      <c r="A133" t="s">
+        <v>49</v>
+      </c>
+      <c r="B133" t="s">
+        <v>19</v>
+      </c>
+      <c r="C133" t="s">
+        <v>36</v>
+      </c>
+      <c r="D133" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5">
+      <c r="A134" t="s">
+        <v>49</v>
+      </c>
+      <c r="B134" t="s">
+        <v>19</v>
+      </c>
+      <c r="C134" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
+      <c r="A135" t="s">
+        <v>49</v>
+      </c>
+      <c r="B135" t="s">
+        <v>12</v>
+      </c>
+      <c r="C135" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
+      <c r="A136" t="s">
+        <v>49</v>
+      </c>
+      <c r="B136" t="s">
+        <v>12</v>
+      </c>
+      <c r="C136" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
+      <c r="A137" t="s">
+        <v>49</v>
+      </c>
+      <c r="B137" t="s">
+        <v>19</v>
+      </c>
+      <c r="C137" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
+      <c r="A138" t="s">
+        <v>49</v>
+      </c>
+      <c r="B138" t="s">
+        <v>10</v>
+      </c>
+      <c r="C138" t="s">
+        <v>13</v>
+      </c>
+      <c r="D138" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
+      <c r="A139" t="s">
+        <v>49</v>
+      </c>
+      <c r="B139" t="s">
+        <v>10</v>
+      </c>
+      <c r="C139" t="s">
+        <v>32</v>
+      </c>
+      <c r="D139" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
+      <c r="A140" t="s">
+        <v>49</v>
+      </c>
+      <c r="B140" t="s">
+        <v>10</v>
+      </c>
+      <c r="C140" t="s">
+        <v>36</v>
+      </c>
+      <c r="D140" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
+      <c r="A141" t="s">
+        <v>49</v>
+      </c>
+      <c r="B141" t="s">
+        <v>10</v>
+      </c>
+      <c r="C141" t="s">
+        <v>37</v>
+      </c>
+      <c r="D141" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
+      <c r="A142" t="s">
         <v>6</v>
       </c>
     </row>
@@ -50881,7 +51128,7 @@
         <v>400001370</v>
       </c>
       <c r="B1992" s="16" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C1992" s="13" t="n">
         <v>119000</v>
@@ -50892,7 +51139,7 @@
         <v>400001964</v>
       </c>
       <c r="B1993" s="16" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C1993" s="13" t="n">
         <v>120000</v>

</xml_diff>